<commit_message>
first running model with output
</commit_message>
<xml_diff>
--- a/GAMS/MakeMeASam.xlsx
+++ b/GAMS/MakeMeASam.xlsx
@@ -1278,7 +1278,7 @@
         <v>13.224999964237215</v>
       </c>
       <c r="AQ29" s="3">
-        <v>935.76332945068134</v>
+        <v>1676.920891655056</v>
       </c>
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.25">
@@ -1292,58 +1292,58 @@
         <v>4</v>
       </c>
       <c r="E30">
-        <v>66.580497209622564</v>
+        <v>49.581221326314676</v>
       </c>
       <c r="F30">
-        <v>5296.2120055640607</v>
+        <v>3437.2150730335607</v>
       </c>
       <c r="G30">
-        <v>112.37468786168873</v>
+        <v>99.154136348548874</v>
       </c>
       <c r="I30">
-        <v>0.93577650262183609</v>
+        <v>0.69685484237796314</v>
       </c>
       <c r="J30">
-        <v>424.95703876860534</v>
+        <v>275.79499036530586</v>
       </c>
       <c r="K30">
-        <v>106.85628801133795</v>
+        <v>94.28496001000407</v>
       </c>
       <c r="M30">
-        <v>41.642054366671708</v>
+        <v>31.01004048581936</v>
       </c>
       <c r="N30">
-        <v>746.88985439225894</v>
+        <v>484.7277757604603</v>
       </c>
       <c r="O30">
-        <v>38.24251264701293</v>
+        <v>33.743393512070234</v>
       </c>
       <c r="P30">
-        <v>160.98474338567453</v>
+        <v>119.88225571273637</v>
       </c>
       <c r="Q30">
-        <v>2107.7941321193125</v>
+        <v>1367.9478378435092</v>
       </c>
       <c r="R30">
-        <v>147.70498259784097</v>
+        <v>130.32792582162438</v>
       </c>
       <c r="T30">
-        <v>43.165270889570401</v>
+        <v>32.144350662446044</v>
       </c>
       <c r="U30">
-        <v>3341.7042243950882</v>
+        <v>2168.7493094392121</v>
       </c>
       <c r="V30">
-        <v>214.03027043433758</v>
+        <v>188.85023861853313</v>
       </c>
       <c r="W30">
-        <v>44.572595780071943</v>
+        <v>33.192358559628047</v>
       </c>
       <c r="X30">
-        <v>866.33087622193693</v>
+        <v>562.24440087671178</v>
       </c>
       <c r="Y30">
-        <v>69.855414565162135</v>
+        <v>61.637130498672462</v>
       </c>
       <c r="AK30">
         <v>2790.021649543196</v>
@@ -1362,6 +1362,9 @@
       </c>
       <c r="AP30">
         <v>1673.4969271477314</v>
+      </c>
+      <c r="AQ30" s="3">
+        <v>2710.1857810455876</v>
       </c>
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.25">
@@ -1404,58 +1407,58 @@
         <v>15</v>
       </c>
       <c r="E32">
-        <v>71.30513385947404</v>
+        <v>53.099567767693429</v>
       </c>
       <c r="F32">
-        <v>6574.4079099172423</v>
+        <v>4266.7578149247265</v>
       </c>
       <c r="G32">
-        <v>69.245983661270103</v>
+        <v>61.099397348179501</v>
       </c>
       <c r="I32">
-        <v>1.0021803918333754</v>
+        <v>0.7463045471099603</v>
       </c>
       <c r="J32">
-        <v>527.51682034635155</v>
+        <v>342.35577508383886</v>
       </c>
       <c r="K32">
-        <v>65.845511249332731</v>
+        <v>58.098980514117116</v>
       </c>
       <c r="M32">
-        <v>44.597027436585201</v>
+        <v>33.210552346393236</v>
       </c>
       <c r="N32">
-        <v>927.14539399002751</v>
+        <v>601.71271840481381</v>
       </c>
       <c r="O32">
-        <v>23.565274852467805</v>
+        <v>20.792889575706887</v>
       </c>
       <c r="P32">
-        <v>172.40842525263676</v>
+        <v>128.38925284770821</v>
       </c>
       <c r="Q32">
-        <v>2616.4923911890301</v>
+        <v>1698.0904608849266</v>
       </c>
       <c r="R32">
-        <v>91.01673167045341</v>
+        <v>80.30888088569418</v>
       </c>
       <c r="T32">
-        <v>46.228333338676855</v>
+        <v>34.42535461390829</v>
       </c>
       <c r="U32">
-        <v>4148.1962320213233</v>
+        <v>2692.158584215545</v>
       </c>
       <c r="V32">
-        <v>131.88678777693059</v>
+        <v>116.3706950972917</v>
       </c>
       <c r="W32">
-        <v>47.735523790935581</v>
+        <v>35.547730482611598</v>
       </c>
       <c r="X32">
-        <v>1075.412494676455</v>
+        <v>697.93732436450227</v>
       </c>
       <c r="Y32">
-        <v>43.045342217849999</v>
+        <v>37.98118430986765</v>
       </c>
       <c r="AK32">
         <v>3792.4625939256516</v>
@@ -1513,70 +1516,70 @@
         <v>1970.0026266263692</v>
       </c>
       <c r="E34">
-        <v>121.3757931389495</v>
+        <v>136.16057952553396</v>
       </c>
       <c r="F34">
-        <v>-210.99953615114583</v>
+        <v>1516.3680487454039</v>
       </c>
       <c r="G34">
-        <v>109.58589703927589</v>
+        <v>118.37613229978382</v>
       </c>
       <c r="H34">
         <v>8270.7683906643706</v>
       </c>
       <c r="I34">
-        <v>1.705914193595153</v>
+        <v>1.9137116159137328</v>
       </c>
       <c r="J34">
-        <v>-16.930164043686247</v>
+        <v>121.67021920595221</v>
       </c>
       <c r="K34">
-        <v>104.20444673824004</v>
+        <v>112.5630186600623</v>
       </c>
       <c r="L34">
         <v>36.801567265183557</v>
       </c>
       <c r="M34">
-        <v>75.91318161498431</v>
+        <v>85.160166908161102</v>
       </c>
       <c r="N34">
-        <v>-29.755873191480994</v>
+        <v>213.84338654545755</v>
       </c>
       <c r="O34">
-        <v>37.293452228466883</v>
+        <v>40.284879297291674</v>
       </c>
       <c r="P34">
-        <v>293.47409122205426</v>
+        <v>329.22217275053418</v>
       </c>
       <c r="Q34">
-        <v>-83.973901292479866</v>
+        <v>603.48635438327244</v>
       </c>
       <c r="R34">
-        <v>144.03940356281402</v>
+        <v>155.59326476492279</v>
       </c>
       <c r="S34">
         <v>161.87206706200377</v>
       </c>
       <c r="T34">
-        <v>78.689994966303985</v>
+        <v>88.27522391723943</v>
       </c>
       <c r="U34">
-        <v>-133.13251821508084</v>
+        <v>956.76938704620022</v>
       </c>
       <c r="V34">
-        <v>208.71870369930497</v>
+        <v>225.4606984117047</v>
       </c>
       <c r="W34">
-        <v>81.255538660743724</v>
+        <v>91.153276510750317</v>
       </c>
       <c r="X34">
-        <v>-34.514368541932299</v>
+        <v>248.04076176792788</v>
       </c>
       <c r="Y34">
-        <v>68.121820081011549</v>
+        <v>73.586089125334553</v>
       </c>
       <c r="AQ34" s="3">
-        <v>11254.516527327865</v>
+        <v>15557.372023099373</v>
       </c>
     </row>
     <row r="35" spans="1:43" x14ac:dyDescent="0.25">
@@ -1593,67 +1596,67 @@
         <v>362.94089424612969</v>
       </c>
       <c r="E35">
-        <v>167.63856968843831</v>
+        <v>188.05862527694231</v>
       </c>
       <c r="F35">
-        <v>-297.96022308015807</v>
+        <v>2141.3192195463084</v>
       </c>
       <c r="G35">
-        <v>156.79343143776526</v>
+        <v>169.37033400348781</v>
       </c>
       <c r="H35">
         <v>4752.6481028090693</v>
       </c>
       <c r="I35">
-        <v>2.3561289119496354</v>
+        <v>2.6431289945983441</v>
       </c>
       <c r="J35">
-        <v>-23.907708743145648</v>
+        <v>171.81500167302804</v>
       </c>
       <c r="K35">
-        <v>149.09375400108931</v>
+        <v>161.05304081581653</v>
       </c>
       <c r="L35">
         <v>99.855379410882833</v>
       </c>
       <c r="M35">
-        <v>104.84773658175878</v>
+        <v>117.61924025962631</v>
       </c>
       <c r="N35">
-        <v>-42.01936542518046</v>
+        <v>301.97612905489319</v>
       </c>
       <c r="O35">
-        <v>53.358766985919566</v>
+        <v>57.638844328798392</v>
       </c>
       <c r="P35">
-        <v>405.33269131150945</v>
+        <v>454.70626986089627</v>
       </c>
       <c r="Q35">
-        <v>-118.58264154711317</v>
+        <v>852.20532735704194</v>
       </c>
       <c r="R35">
-        <v>206.08885775482912</v>
+        <v>222.61990411369615</v>
       </c>
       <c r="S35">
         <v>306.43795562512798</v>
       </c>
       <c r="T35">
-        <v>108.68294133279251</v>
+        <v>121.92161133374998</v>
       </c>
       <c r="U35">
-        <v>-188.00133663883071</v>
+        <v>1351.0893208615421</v>
       </c>
       <c r="V35">
-        <v>298.63077861677061</v>
+        <v>322.58490839981425</v>
       </c>
       <c r="W35">
-        <v>112.22635031317063</v>
+        <v>125.89664299193191</v>
       </c>
       <c r="X35">
-        <v>-48.739012122084667</v>
+        <v>350.26750322523304</v>
       </c>
       <c r="Y35">
-        <v>97.467413370351323</v>
+        <v>105.28558630050034</v>
       </c>
     </row>
     <row r="36" spans="1:43" x14ac:dyDescent="0.25">
@@ -1693,13 +1696,13 @@
         <v>10054.140996092767</v>
       </c>
       <c r="AH37">
-        <v>3398.4930289857666</v>
+        <v>4697.8135614675411</v>
       </c>
       <c r="AI37">
-        <v>389.41267229217522</v>
+        <v>2861.6890730728678</v>
       </c>
       <c r="AQ37" s="3">
-        <v>-2985.6090829600616</v>
+        <v>-6757.206016222528</v>
       </c>
     </row>
     <row r="38" spans="1:43" x14ac:dyDescent="0.25">
@@ -1716,13 +1719,13 @@
         <v>16661.914502887495</v>
       </c>
       <c r="AH38">
-        <v>861.58978199639159</v>
+        <v>1190.9949874143063</v>
       </c>
       <c r="AI38">
-        <v>4880.1902769789622</v>
+        <v>5088.1592742925122</v>
       </c>
       <c r="AQ38" s="3">
-        <v>-13458.859692591614</v>
+        <v>-13996.233895323079</v>
       </c>
     </row>
     <row r="39" spans="1:43" x14ac:dyDescent="0.25">
@@ -1739,13 +1742,13 @@
         <v>110.55457677839405</v>
       </c>
       <c r="AH39">
-        <v>1914.6439599919813</v>
+        <v>2646.655527587347</v>
       </c>
       <c r="AI39">
-        <v>216.04251755338072</v>
+        <v>577.08959305420069</v>
       </c>
       <c r="AQ39" s="3">
-        <v>2398.7180793022058</v>
+        <v>1305.65943620602</v>
       </c>
     </row>
     <row r="40" spans="1:43" x14ac:dyDescent="0.25">
@@ -1759,13 +1762,13 @@
         <v>9</v>
       </c>
       <c r="AH40">
-        <v>5079.7897563537254</v>
+        <v>7021.90794663018</v>
       </c>
       <c r="AI40">
-        <v>492.83890751922542</v>
+        <v>1529.5315013316342</v>
       </c>
       <c r="AQ40" s="3">
-        <v>4892.8030258032959</v>
+        <v>1913.9922417144317</v>
       </c>
     </row>
     <row r="41" spans="1:43" x14ac:dyDescent="0.25">
@@ -1782,13 +1785,13 @@
         <v>158.60476837297716</v>
       </c>
       <c r="AH41">
-        <v>6323.1314861423352</v>
+        <v>8740.6072612739426</v>
       </c>
       <c r="AI41">
-        <v>525.75033893586033</v>
+        <v>2102.0337962202343</v>
       </c>
       <c r="AQ41" s="3">
-        <v>2005.9083489067307</v>
+        <v>-1987.8508835092507</v>
       </c>
     </row>
     <row r="42" spans="1:43" x14ac:dyDescent="0.25">
@@ -1802,13 +1805,13 @@
         <v>11</v>
       </c>
       <c r="AH42">
-        <v>4931.3850411855301</v>
+        <v>6816.7647618254314</v>
       </c>
       <c r="AI42">
-        <v>160.95475156143729</v>
+        <v>581.44973251766532</v>
       </c>
       <c r="AQ42" s="3">
-        <v>-209.59528114836303</v>
+        <v>-2515.469982744492</v>
       </c>
     </row>
     <row r="43" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1827,14 +1830,11 @@
       <c r="AA43" s="3">
         <v>4150.2884720414877</v>
       </c>
-      <c r="AD43" s="3">
-        <v>16771.689338838572</v>
-      </c>
       <c r="AE43" s="3">
-        <v>3414.6992680652734</v>
+        <v>2301.0294805195881</v>
       </c>
       <c r="AF43" s="3">
-        <v>13339.606041531195</v>
+        <v>24298.689509745833</v>
       </c>
       <c r="AJ43" s="3">
         <v>41052.959415035271</v>

</xml_diff>